<commit_message>
Fixed part orientations for production.
</commit_message>
<xml_diff>
--- a/fixed/radial_18mA/production/ver_0p1_rev_1/CPL_JLCPCB_radial_18mA.xlsx
+++ b/fixed/radial_18mA/production/ver_0p1_rev_1/CPL_JLCPCB_radial_18mA.xlsx
@@ -217,7 +217,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -348,7 +348,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -365,7 +365,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -382,7 +382,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>